<commit_message>
change from z to t dist
</commit_message>
<xml_diff>
--- a/step2-Count.xlsx
+++ b/step2-Count.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Serkan\git\IE306Assignment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD8F113-A074-4ECD-BDFA-4E2FABF2EA88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBF2D2D-11FB-43BB-BCE1-EA3D8A683CBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="23900" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,8 +105,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -451,7 +454,7 @@
   <dimension ref="A1:M91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8:K8"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -575,12 +578,12 @@
       <c r="I6" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -607,15 +610,15 @@
         <v>17.100000000000001</v>
       </c>
       <c r="J7" s="1">
-        <f>I7-1.96*H7/SQRT(30)</f>
-        <v>12.281236157942867</v>
-      </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1">
-        <f>I7+1.96*H7/SQRT(30)</f>
-        <v>21.918763842057135</v>
-      </c>
-      <c r="M7" s="1"/>
+        <f>I7-2.045*H7/SQRT(30)</f>
+        <v>12.072259154588348</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2">
+        <f>I7+2.045*H7/SQRT(30)</f>
+        <v>22.127740845411655</v>
+      </c>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -642,15 +645,15 @@
         <v>13.933333333333334</v>
       </c>
       <c r="J8" s="1">
-        <f>I8-1.96*H8/SQRT(30)</f>
-        <v>9.4382978359645566</v>
-      </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1">
-        <f>I8+1.96*H8/SQRT(30)</f>
-        <v>18.428368830702112</v>
-      </c>
-      <c r="M8" s="1"/>
+        <f t="shared" ref="J8:J9" si="0">I8-2.045*H8/SQRT(30)</f>
+        <v>9.2433600720480538</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2">
+        <f t="shared" ref="L8:L9" si="1">I8+2.045*H8/SQRT(30)</f>
+        <v>18.623306594618612</v>
+      </c>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -677,15 +680,15 @@
         <v>17.566666666666666</v>
       </c>
       <c r="J9" s="1">
-        <f>I9-1.96*H9/SQRT(30)</f>
-        <v>13.004843372964579</v>
-      </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1">
-        <f>I9+1.96*H9/SQRT(30)</f>
-        <v>22.128489960368753</v>
-      </c>
-      <c r="M9" s="1"/>
+        <f t="shared" si="0"/>
+        <v>12.807009199513214</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2">
+        <f t="shared" si="1"/>
+        <v>22.326324133820119</v>
+      </c>
+      <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">

</xml_diff>